<commit_message>
model: add v4.0.5 Qair model
</commit_message>
<xml_diff>
--- a/resources/config/deployment_list.xlsx
+++ b/resources/config/deployment_list.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.gruet\Code\ems-optimizer\optimAnalyser\data_cplex\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.gruet\Code\ems-optim-analyser\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6A1380BC-DB2A-48E7-8189-4ACA2266351F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2291D18B-B753-4213-BE47-83B082797762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{BEC0A7A9-D060-4CC7-A263-5E7F9B7FC146}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{BEC0A7A9-D060-4CC7-A263-5E7F9B7FC146}"/>
   </bookViews>
   <sheets>
     <sheet name="DEPLOYMENTS_PROD" sheetId="2" r:id="rId1"/>
@@ -571,13 +571,13 @@
     <t>MICROGRID_QAIR</t>
   </si>
   <si>
-    <t>MicrogridOptimizer 20.mod</t>
-  </si>
-  <si>
-    <t>MicrogridOptimizer 20</t>
-  </si>
-  <si>
     <t>HIL_2</t>
+  </si>
+  <si>
+    <t>Microgrid_Optimizer_V4.0.5_QairMU_XL5</t>
+  </si>
+  <si>
+    <t>Microgrid_Optimizer_V4.0.5_QairMU_XL5.mod</t>
   </si>
 </sst>
 </file>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E443281-2889-4F20-947F-4026A0971884}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A23" zoomScale="56" workbookViewId="0">
-      <selection activeCell="B35" sqref="B35"/>
+    <sheetView topLeftCell="A23" zoomScale="56" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1949,7 +1949,7 @@
         <v>1802</v>
       </c>
       <c r="B35" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C35" t="s">
         <v>45</v>
@@ -1992,7 +1992,7 @@
   <dimension ref="A1:E36"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D37" sqref="D37"/>
+      <selection activeCell="D36" sqref="D36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -2461,7 +2461,7 @@
         <v>46</v>
       </c>
       <c r="D36" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
     </row>
   </sheetData>
@@ -2480,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00E7692-29CE-4D37-AEFD-C4BEE531BC29}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2521,15 +2521,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_ip_UnifiedCompliancePolicyUIAction xmlns="http://schemas.microsoft.com/sharepoint/v3" xsi:nil="true"/>
@@ -2540,6 +2531,15 @@
     </lcf76f155ced4ddcb4097134ff3c332f>
   </documentManagement>
 </p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2815,14 +2815,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE6D975-0C61-4E06-890E-C1257119A4ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9177F04-86DD-420E-9832-D1F1887B5BC2}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -2830,6 +2822,14 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3"/>
     <ds:schemaRef ds:uri="c0561af2-392e-4b97-a94a-1399528930a0"/>
     <ds:schemaRef ds:uri="1cb02928-68ea-4f70-8d23-1dcfa67d5431"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE6D975-0C61-4E06-890E-C1257119A4ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>

</xml_diff>

<commit_message>
model: Qair_v4.0.5 update model ID
</commit_message>
<xml_diff>
--- a/resources/config/deployment_list.xlsx
+++ b/resources/config/deployment_list.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\quentin.gruet\Code\ems-optim-analyser\resources\config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2291D18B-B753-4213-BE47-83B082797762}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92CDB374-1DAC-4B53-885D-CA2AE7D4FF29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{BEC0A7A9-D060-4CC7-A263-5E7F9B7FC146}"/>
+    <workbookView xWindow="-105" yWindow="-16320" windowWidth="29040" windowHeight="15720" xr2:uid="{BEC0A7A9-D060-4CC7-A263-5E7F9B7FC146}"/>
   </bookViews>
   <sheets>
     <sheet name="DEPLOYMENTS_PROD" sheetId="2" r:id="rId1"/>
@@ -1196,8 +1196,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E443281-2889-4F20-947F-4026A0971884}">
   <dimension ref="A1:I36"/>
   <sheetViews>
-    <sheetView topLeftCell="A23" zoomScale="56" workbookViewId="0">
-      <selection activeCell="F36" sqref="F36"/>
+    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="56" workbookViewId="0">
+      <selection activeCell="A37" sqref="A37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5"/>
@@ -1963,7 +1963,7 @@
     </row>
     <row r="36" spans="1:7">
       <c r="A36">
-        <v>1694</v>
+        <v>1799</v>
       </c>
       <c r="B36" t="s">
         <v>176</v>
@@ -2480,7 +2480,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E00E7692-29CE-4D37-AEFD-C4BEE531BC29}">
   <dimension ref="A1:A5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A10" sqref="A10"/>
     </sheetView>
   </sheetViews>
@@ -2534,15 +2534,6 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100F6EB266767B42549B9F3FD0AE2922999" ma:contentTypeVersion="22" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="e25bd20e13b7c1b7f26102be0f5125ed">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns1="http://schemas.microsoft.com/sharepoint/v3" xmlns:ns2="1cb02928-68ea-4f70-8d23-1dcfa67d5431" xmlns:ns3="c0561af2-392e-4b97-a94a-1399528930a0" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="4b296ce92c881bae9fc9507e1510730d" ns1:_="" ns2:_="" ns3:_="">
     <xsd:import namespace="http://schemas.microsoft.com/sharepoint/v3"/>
@@ -2814,6 +2805,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B9177F04-86DD-420E-9832-D1F1887B5BC2}">
   <ds:schemaRefs>
@@ -2827,14 +2827,6 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE6D975-0C61-4E06-890E-C1257119A4ED}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B334646A-1D03-40DF-A64D-1FA27974817B}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2852,4 +2844,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3CE6D975-0C61-4E06-890E-C1257119A4ED}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>